<commit_message>
Refatoração no caminho que está genérico, criação de um parametro para saber se o teste passou ou não e ajustes no screenshot
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA709640-2C70-4F18-9669-6BF788F0595A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCF6E2D-98E5-4EAB-BB88-379DC308E35E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastro" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -79,9 +79,6 @@
     <t>06784-200</t>
   </si>
   <si>
-    <t>FLP00</t>
-  </si>
-  <si>
     <t>Felipe2</t>
   </si>
   <si>
@@ -89,12 +86,25 @@
   </si>
   <si>
     <t>Brazil</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Reprovado</t>
+  </si>
+  <si>
+    <t>BRUN227</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -433,29 +443,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="22.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="28.5703125" collapsed="true"/>
+    <col min="3" max="4" style="2" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="10.5703125" collapsed="true"/>
+    <col min="14" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,19 +503,22 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -513,10 +527,10 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
@@ -530,19 +544,22 @@
       <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -551,10 +568,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
@@ -567,6 +584,9 @@
       </c>
       <c r="L3" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refatoração de código, excluindo classes em não utilizadas
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCF6E2D-98E5-4EAB-BB88-379DC308E35E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8009338-E54E-4C6C-A88A-8BD2C3148AA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastro" sheetId="1" r:id="rId1"/>
+    <sheet name="buscar" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -98,14 +99,25 @@
   </si>
   <si>
     <t>Aprovado</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>HP CHROMEBOOK 14 G1 (ENERGY STAR)</t>
+  </si>
+  <si>
+    <t>HP CHROMEBOOK 14 G1 (ES)</t>
+  </si>
+  <si>
+    <t>HP ENVY - PORTÁTIL TOQUE 17T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +137,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF2A2A2A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,6 +180,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -445,25 +468,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="22.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="28.5703125" collapsed="true"/>
-    <col min="3" max="4" style="2" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="10.5703125" collapsed="true"/>
-    <col min="14" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="9.140625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -597,4 +620,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508EA9C3-02BD-4BFE-A2FC-3E0A1F9398A0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refatoração no uso do sleep, que foi substituido pelo metodo until da classe Wait
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8009338-E54E-4C6C-A88A-8BD2C3148AA0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D7EE59-F731-40EF-8747-60739ACC0FBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="cadastro" sheetId="1" r:id="rId1"/>
-    <sheet name="buscar" sheetId="2" r:id="rId2"/>
+    <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
+    <sheet name="CadastroFalha" sheetId="3" r:id="rId2"/>
+    <sheet name="buscar" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -92,15 +93,9 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>Reprovado</t>
-  </si>
-  <si>
     <t>BRUN227</t>
   </si>
   <si>
-    <t>Aprovado</t>
-  </si>
-  <si>
     <t>Modelo</t>
   </si>
   <si>
@@ -111,6 +106,21 @@
   </si>
   <si>
     <t>HP ENVY - PORTÁTIL TOQUE 17T</t>
+  </si>
+  <si>
+    <t>BRUN229</t>
+  </si>
+  <si>
+    <t>felipe</t>
+  </si>
+  <si>
+    <t>almeida</t>
+  </si>
+  <si>
+    <t>BRUN230</t>
+  </si>
+  <si>
+    <t>BRUN231</t>
   </si>
 </sst>
 </file>
@@ -468,25 +478,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.140625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="37" style="2" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -532,7 +543,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -567,13 +578,11 @@
       <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
+      <c r="M2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>12</v>
@@ -608,9 +617,7 @@
       <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
-        <v>23</v>
-      </c>
+      <c r="M3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -623,10 +630,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB2D1F4-E107-4B1A-B01B-C8B4CC597D7B}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="37" style="2" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="2" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3E3F0085-1FE4-4463-8559-4B911B0C1EA8}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{B5CE8F94-96E0-47B0-9E6D-9E23AC32E85B}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508EA9C3-02BD-4BFE-A2FC-3E0A1F9398A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -638,7 +799,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -646,17 +807,17 @@
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementação de teste com falha, para o teste passar as senhasnão devem ser iguais e nem o botão ativo
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA11662F-A35D-475A-9705-1B542F6353A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457AA23D-71BE-4D1F-839E-D59715A3691C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>BRUN227</t>
-  </si>
-  <si>
     <t>Modelo</t>
   </si>
   <si>
@@ -105,12 +102,6 @@
     <t>HP ENVY - PORTÁTIL TOQUE 17T</t>
   </si>
   <si>
-    <t>BRUN229</t>
-  </si>
-  <si>
-    <t>felipe</t>
-  </si>
-  <si>
     <t>almeida</t>
   </si>
   <si>
@@ -120,7 +111,13 @@
     <t>Rua Bueno, 188</t>
   </si>
   <si>
-    <t>BRUN259</t>
+    <t>BRUN260</t>
+  </si>
+  <si>
+    <t>BRUN262</t>
+  </si>
+  <si>
+    <t>Felipe3</t>
   </si>
 </sst>
 </file>
@@ -478,7 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -543,7 +540,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -561,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
@@ -570,7 +567,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>17</v>
@@ -596,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB2D1F4-E107-4B1A-B01B-C8B4CC597D7B}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,13 +658,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -679,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
@@ -699,48 +696,12 @@
       <c r="M2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="M3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3E3F0085-1FE4-4463-8559-4B911B0C1EA8}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{B5CE8F94-96E0-47B0-9E6D-9E23AC32E85B}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -762,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -770,17 +731,17 @@
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementando teste de busca pela home page
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457AA23D-71BE-4D1F-839E-D59715A3691C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA2275-AC92-43A9-A12B-5902EA076BC9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
     <sheet name="CadastroFalha" sheetId="3" r:id="rId2"/>
-    <sheet name="buscar" sheetId="2" r:id="rId3"/>
+    <sheet name="buscarHome" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -93,15 +93,6 @@
     <t>Modelo</t>
   </si>
   <si>
-    <t>HP CHROMEBOOK 14 G1 (ENERGY STAR)</t>
-  </si>
-  <si>
-    <t>HP CHROMEBOOK 14 G1 (ES)</t>
-  </si>
-  <si>
-    <t>HP ENVY - PORTÁTIL TOQUE 17T</t>
-  </si>
-  <si>
     <t>almeida</t>
   </si>
   <si>
@@ -118,6 +109,9 @@
   </si>
   <si>
     <t>Felipe3</t>
+  </si>
+  <si>
+    <t>BOSE SOUNDLINK BLUETOOTH SPEAKER III</t>
   </si>
 </sst>
 </file>
@@ -177,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,6 +185,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -540,7 +537,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -558,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
@@ -567,7 +564,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>17</v>
@@ -593,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB2D1F4-E107-4B1A-B01B-C8B4CC597D7B}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -658,13 +655,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -676,7 +673,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
@@ -711,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508EA9C3-02BD-4BFE-A2FC-3E0A1F9398A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,19 +727,15 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>23</v>
+      <c r="A2" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="A3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Implantação da busca pela home com sucesso através de massa de dados
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA2275-AC92-43A9-A12B-5902EA076BC9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654FFD0A-54B2-41B1-88AF-D8B8C6046F53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-90" windowWidth="15600" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
     <sheet name="CadastroFalha" sheetId="3" r:id="rId2"/>
-    <sheet name="buscarHome" sheetId="2" r:id="rId3"/>
+    <sheet name="buscarHomeSucesso" sheetId="2" r:id="rId3"/>
+    <sheet name="buscarHomeFail" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -111,7 +112,7 @@
     <t>Felipe3</t>
   </si>
   <si>
-    <t>BOSE SOUNDLINK BLUETOOTH SPEAKER III</t>
+    <t>Bose Soundlink Bluetooth Speaker III</t>
   </si>
 </sst>
 </file>
@@ -706,10 +707,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508EA9C3-02BD-4BFE-A2FC-3E0A1F9398A0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,27 +719,36 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B601A69-DC0F-4ED2-9E8A-6A113BE67791}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implantação da busca pela home com falha com try/catch
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654FFD0A-54B2-41B1-88AF-D8B8C6046F53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD91390-B88A-46F3-B593-47F8415AAFD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-90" windowWidth="15600" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
     <sheet name="CadastroFalha" sheetId="3" r:id="rId2"/>
     <sheet name="buscarHomeSucesso" sheetId="2" r:id="rId3"/>
-    <sheet name="buscarHomeFail" sheetId="4" r:id="rId4"/>
+    <sheet name="buscarHomeFalha" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Bose Soundlink Bluetooth Speaker III</t>
+  </si>
+  <si>
+    <t>Dell Vostro</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +192,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -710,7 +716,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,12 +749,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B601A69-DC0F-4ED2-9E8A-6A113BE67791}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refatoração, criando pageActions e iniciando Busca pela barra de pesquisa
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD91390-B88A-46F3-B593-47F8415AAFD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9885DB36-9338-42C7-8135-11253AE38F20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-90" windowWidth="15600" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-90" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
     <sheet name="CadastroFalha" sheetId="3" r:id="rId2"/>
     <sheet name="buscarHomeSucesso" sheetId="2" r:id="rId3"/>
     <sheet name="buscarHomeFalha" sheetId="4" r:id="rId4"/>
+    <sheet name="BuscaBarraSucesso" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -106,9 +107,6 @@
     <t>BRUN260</t>
   </si>
   <si>
-    <t>BRUN262</t>
-  </si>
-  <si>
     <t>Felipe3</t>
   </si>
   <si>
@@ -116,13 +114,19 @@
   </si>
   <si>
     <t>Dell Vostro</t>
+  </si>
+  <si>
+    <t>HP USB 3 Button Optical Mouse</t>
+  </si>
+  <si>
+    <t>BRUN268</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +157,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -175,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -479,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -544,7 +555,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -668,7 +679,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -732,7 +743,7 @@
     </row>
     <row r="2" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -751,9 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B601A69-DC0F-4ED2-9E8A-6A113BE67791}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -767,6 +776,35 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D9AC-DF87-4EEE-9FC0-7844A5C7A27A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implantação da Busca em barra de pesquisa com falha e sucesso
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9885DB36-9338-42C7-8135-11253AE38F20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97112B72-93D4-4F45-8B88-77872ED68D38}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-90" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="buscarHomeSucesso" sheetId="2" r:id="rId3"/>
     <sheet name="buscarHomeFalha" sheetId="4" r:id="rId4"/>
     <sheet name="BuscaBarraSucesso" sheetId="5" r:id="rId5"/>
+    <sheet name="BuscaBarraFalha" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -120,6 +121,9 @@
   </si>
   <si>
     <t>BRUN268</t>
+  </si>
+  <si>
+    <t>Mouse Dell Supra</t>
   </si>
 </sst>
 </file>
@@ -490,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -789,9 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D9AC-DF87-4EEE-9FC0-7844A5C7A27A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -812,4 +814,32 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E9CAA3-701D-40B5-9EDB-AD35447A9B38}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implantação de cenário completo, até a compra efetuada
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97112B72-93D4-4F45-8B88-77872ED68D38}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034FF75B-033E-4544-9E7F-1079FD0604D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -124,13 +124,19 @@
   </si>
   <si>
     <t>Mouse Dell Supra</t>
+  </si>
+  <si>
+    <t>BRUN255</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +173,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -185,11 +198,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,10 +225,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,10 +746,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508EA9C3-02BD-4BFE-A2FC-3E0A1F9398A0}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,20 +758,26 @@
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
     </row>
   </sheetData>
@@ -791,23 +815,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D9AC-DF87-4EEE-9FC0-7844A5C7A27A}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -818,28 +850,47 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E9CAA3-701D-40B5-9EDB-AD35447A9B38}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exclusão das PageActions, criação do DriverFactory e modificando a forma em que clicamos nos métodos pela PageFactory
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034FF75B-033E-4544-9E7F-1079FD0604D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6626BA-71AF-4A14-A38E-788BB5B52A0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -120,13 +120,13 @@
     <t>HP USB 3 Button Optical Mouse</t>
   </si>
   <si>
-    <t>BRUN268</t>
-  </si>
-  <si>
     <t>Mouse Dell Supra</t>
   </si>
   <si>
     <t>BRUN255</t>
+  </si>
+  <si>
+    <t>BRUN294</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -577,7 +577,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -768,7 +768,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -817,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D9AC-DF87-4EEE-9FC0-7844A5C7A27A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
@@ -836,7 +836,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refatoração no classe DriverFactory
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6626BA-71AF-4A14-A38E-788BB5B52A0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EC1A41-5138-4586-876E-929BCB51A56D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
     <t>BRUN255</t>
   </si>
   <si>
-    <t>BRUN294</t>
+    <t>BRUN295</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refatoração no cenário de teste de busca pela home
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EC1A41-5138-4586-876E-929BCB51A56D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8ED6FF-6857-454A-81E3-F362E450C829}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <t>BRUN255</t>
   </si>
   <si>
-    <t>BRUN295</t>
+    <t>BRUN409</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refatoração na classe HomePage
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8ED6FF-6857-454A-81E3-F362E450C829}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EAC1E3-DCC0-4627-B4CD-E6800E68B1FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <t>BRUN255</t>
   </si>
   <si>
-    <t>BRUN409</t>
+    <t>BRUN410</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Adicionando Managers e configurações ao TDD, usando Singletton
</commit_message>
<xml_diff>
--- a/MassaDados.xlsx
+++ b/MassaDados.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EAC1E3-DCC0-4627-B4CD-E6800E68B1FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9C9B9E-E6AE-4154-AF4F-6664003326FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastroSucesso" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <t>BRUN255</t>
   </si>
   <si>
-    <t>BRUN410</t>
+    <t>BRUN411</t>
   </si>
 </sst>
 </file>

</xml_diff>